<commit_message>
Changes and added some pages
</commit_message>
<xml_diff>
--- a/com.AE_Management/src/main/resources/Data/Login.xlsx
+++ b/com.AE_Management/src/main/resources/Data/Login.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkInno\Poonam\TestingCodeRepositry\Automation-coding-Task\com.AE_Management\src\main\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F470BBFE-1056-48AF-878B-5CCC02AE65BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C1F2890-23DD-48C5-BBF9-65E01ABF992B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>VesselAECode</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>FAIJ</t>
+  </si>
+  <si>
+    <t>Test Baltic Spirit</t>
+  </si>
+  <si>
+    <t>TBSJ</t>
   </si>
 </sst>
 </file>
@@ -160,9 +166,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -200,7 +206,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -306,7 +312,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -448,7 +454,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -456,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -484,6 +490,14 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>